<commit_message>
Electronic: BOM (add 3V3 & 5V Regulator) + PowerCalc (add discharge path)
</commit_message>
<xml_diff>
--- a/Electronic/Design/Power_Calc.xlsx
+++ b/Electronic/Design/Power_Calc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
   <si>
     <t>V</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>https://www.digikey.de/product-detail/de/analog-devices-inc/LT1374CS8-5-PBF/LT1374CS8-5-PBF-ND/888771</t>
+  </si>
+  <si>
+    <t>Battery &amp; Protection Circuit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L = </t>
+  </si>
+  <si>
+    <t>10-22 uH</t>
+  </si>
+  <si>
+    <t>Max. 8.4V</t>
   </si>
 </sst>
 </file>
@@ -106,7 +118,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +136,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -356,10 +376,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -422,6 +443,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,9 +468,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -470,6 +497,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>43887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18640425" y="800100"/>
+          <a:ext cx="4438650" cy="2148912"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>543506</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163339</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14058900" y="3886200"/>
+          <a:ext cx="3572456" cy="2125489"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -735,414 +843,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="H3:Y24"/>
+  <dimension ref="A3:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="12.21875" customWidth="1"/>
-    <col min="10" max="11" width="14.44140625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" customWidth="1"/>
-    <col min="15" max="15" width="4.5546875" customWidth="1"/>
-    <col min="19" max="19" width="4.33203125" customWidth="1"/>
-    <col min="20" max="20" width="4.6640625" customWidth="1"/>
-    <col min="21" max="21" width="4.109375" customWidth="1"/>
-    <col min="22" max="22" width="5.77734375" customWidth="1"/>
-    <col min="23" max="23" width="4.21875" customWidth="1"/>
-    <col min="24" max="24" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" customWidth="1"/>
+    <col min="15" max="15" width="4.140625" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="55"/>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="8:24" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="8:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H4" s="44" t="s">
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="45"/>
-      <c r="K4" s="50" t="s">
+      <c r="C4" s="46"/>
+      <c r="E4" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="P4" s="48" t="s">
+      <c r="H4" s="1"/>
+      <c r="J4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="H5" s="32">
+      <c r="K4" s="50"/>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="32">
         <v>6</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="51"/>
-      <c r="N5" s="4">
+      <c r="E5" s="52"/>
+      <c r="H5" s="4">
         <v>6</v>
       </c>
-      <c r="O5" t="s">
+      <c r="I5" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="7">
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7">
         <v>3.3</v>
       </c>
-      <c r="S5" t="s">
+      <c r="M5" t="s">
         <v>0</v>
       </c>
-      <c r="T5" s="11"/>
-      <c r="U5">
+      <c r="N5" s="11"/>
+      <c r="O5">
         <v>1</v>
       </c>
-      <c r="V5" s="2">
+      <c r="P5" s="2">
         <v>40</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Q5" t="s">
         <v>1</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="8:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H6" s="34">
+      <c r="T5" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="U5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="34">
+        <f>B7/B5</f>
+        <v>4.5391755532622398</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="8">
         <f>H7/H5</f>
-        <v>4.5391755532622398</v>
-      </c>
-      <c r="I6" s="33" t="s">
+        <v>124.47368421052632</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="11">
+        <v>95</v>
+      </c>
+      <c r="L6" s="12">
+        <f>O5*P5+O6*P6+O7*P7+O8*P8</f>
+        <v>215</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="O6" s="31">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="35">
+        <f>SUM(H7,H22)/(E10/100)/1000</f>
+        <v>27.235053319573439</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="29"/>
+      <c r="H7" s="4">
+        <f>L7*100/K6</f>
+        <v>746.84210526315792</v>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="7">
+        <f>(L6*L5)</f>
+        <v>709.5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36"/>
+      <c r="C8" s="9"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="30"/>
+      <c r="H8" s="16">
+        <f>H7-L7</f>
+        <v>37.342105263157919</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="N8" s="11"/>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="37">
+        <f>B7-(H7+H22)/1000</f>
+        <v>2.723505331957341</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E10" s="24">
+        <v>90</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="H10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E11" s="23"/>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="40"/>
+      <c r="C13" s="39"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E15" s="23"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E16" s="23"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E17" s="26"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="23"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="27"/>
+      <c r="F19" s="11"/>
+      <c r="H19" s="1"/>
+      <c r="J19" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="H20" s="4">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="5"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="7">
+        <v>5</v>
+      </c>
+      <c r="M20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="11"/>
+      <c r="H21" s="19">
+        <f>H22/H20</f>
+        <v>3960.7843137254899</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="11">
+        <v>85</v>
+      </c>
+      <c r="L21" s="20">
+        <f>(P21*O21+P22*O22)</f>
+        <v>4040</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="15"/>
+      <c r="O21" s="31">
+        <v>2</v>
+      </c>
+      <c r="P21" s="21">
+        <v>1920</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="S21" t="s">
+        <v>20</v>
+      </c>
+      <c r="T21" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="U21">
+        <f>(0.29*L20*(H20+2.4-L20))/(0.2*500000*(H20+2.4))</f>
+        <v>5.8690476190476194E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="11"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="4">
+        <f>L22*100/K21</f>
+        <v>23764.705882352941</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="28"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="7">
+        <f>L21*L20</f>
+        <v>20200</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" s="11"/>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22" s="21">
+        <v>200</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="11"/>
+      <c r="H23" s="16">
+        <f>H22-L22</f>
+        <v>3564.7058823529405</v>
+      </c>
+      <c r="I23" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="46"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="32">
+        <v>6</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="52"/>
+      <c r="F26" s="53"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="34">
+        <f>B28/B26</f>
+        <v>4.085257997936016</v>
+      </c>
+      <c r="C27" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="8">
-        <f>N7/N5</f>
-        <v>124.47368421052632</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="P6" s="10" t="s">
+      <c r="D27" s="15"/>
+      <c r="E27" s="52"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="35">
+        <f>SUM(H7,H22)/(E30/100)/1000</f>
+        <v>24.511547987616098</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="52"/>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="36"/>
+      <c r="C29" s="9"/>
+      <c r="E29" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Q6" s="11">
-        <v>95</v>
-      </c>
-      <c r="R6" s="12">
-        <f>U5*V5+U6*V6+U7*V7+U8*V8</f>
-        <v>215</v>
-      </c>
-      <c r="S6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="T6" s="15"/>
-      <c r="U6" s="31">
-        <v>1</v>
-      </c>
-      <c r="V6" s="2">
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="37">
+        <f>B28-(H7+H22)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E31" s="23"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="E32" s="24"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="25"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="23"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="23"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="23"/>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="27"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="48"/>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="41">
+        <f>B9+(H8+H23)/1000</f>
+        <v>6.325553319573439</v>
+      </c>
+      <c r="C47" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="W6" t="s">
-        <v>1</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="8:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H7" s="35">
-        <f>SUM(N7,N22)/(K10/100)/1000</f>
-        <v>27.235053319573439</v>
-      </c>
-      <c r="I7" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="51"/>
-      <c r="L7" s="29"/>
-      <c r="N7" s="4">
-        <f>R7*100/Q6</f>
-        <v>746.84210526315792</v>
-      </c>
-      <c r="O7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="7">
-        <f>(R6*R5)</f>
-        <v>709.5</v>
-      </c>
-      <c r="S7" t="s">
-        <v>2</v>
-      </c>
-      <c r="T7" s="11"/>
-      <c r="U7">
-        <v>4</v>
-      </c>
-      <c r="V7" s="2">
-        <v>20</v>
-      </c>
-      <c r="W7" t="s">
-        <v>1</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="8:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H8" s="36"/>
-      <c r="I8" s="9"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="30"/>
-      <c r="N8" s="16">
-        <f>N7-R7</f>
-        <v>37.342105263157919</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="P8" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="R8" s="1"/>
-      <c r="T8" s="11"/>
-      <c r="U8">
-        <v>4</v>
-      </c>
-      <c r="V8" s="2">
-        <v>20</v>
-      </c>
-      <c r="W8" t="s">
-        <v>1</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="H9" s="37">
-        <f>H7-(N7+N22)/1000</f>
-        <v>2.723505331957341</v>
-      </c>
-      <c r="I9" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="30"/>
-      <c r="P9" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="K10" s="24">
-        <v>90</v>
-      </c>
-      <c r="L10" s="30"/>
-      <c r="N10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-    </row>
-    <row r="11" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="K11" s="23"/>
-      <c r="L11" s="30"/>
-    </row>
-    <row r="12" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="30"/>
-    </row>
-    <row r="13" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="H13" s="40"/>
-      <c r="I13" s="39"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="30"/>
-    </row>
-    <row r="14" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="30"/>
-    </row>
-    <row r="15" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="K15" s="23"/>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="8:24" x14ac:dyDescent="0.3">
-      <c r="K16" s="23"/>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" spans="8:25" x14ac:dyDescent="0.3">
-      <c r="K17" s="26"/>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="18" spans="8:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K18" s="23"/>
-      <c r="L18" s="11"/>
-    </row>
-    <row r="19" spans="8:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K19" s="27"/>
-      <c r="L19" s="11"/>
-      <c r="N19" s="1"/>
-      <c r="P19" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="1"/>
-    </row>
-    <row r="20" spans="8:25" x14ac:dyDescent="0.3">
-      <c r="K20" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="11"/>
-      <c r="N20" s="4">
-        <v>6</v>
-      </c>
-      <c r="O20" t="s">
-        <v>0</v>
-      </c>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="7">
-        <v>5</v>
-      </c>
-      <c r="S20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="8:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="L21" s="11"/>
-      <c r="N21" s="19">
-        <f>N22/N20</f>
-        <v>3960.7843137254899</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="P21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q21" s="11">
-        <v>85</v>
-      </c>
-      <c r="R21" s="20">
-        <f>(V21*U21+V22*U22)</f>
-        <v>4040</v>
-      </c>
-      <c r="S21" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="T21" s="15"/>
-      <c r="U21" s="31">
-        <v>2</v>
-      </c>
-      <c r="V21" s="21">
-        <v>1920</v>
-      </c>
-      <c r="W21" t="s">
-        <v>1</v>
-      </c>
-      <c r="X21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="8:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="M22" s="52"/>
-      <c r="N22" s="4">
-        <f>R22*100/Q21</f>
-        <v>23764.705882352941</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P22" s="28"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="7">
-        <f>R21*R20</f>
-        <v>20200</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T22" s="11"/>
-      <c r="U22">
-        <v>1</v>
-      </c>
-      <c r="V22" s="21">
-        <v>200</v>
-      </c>
-      <c r="W22" t="s">
-        <v>1</v>
-      </c>
-      <c r="X22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="8:25" x14ac:dyDescent="0.3">
-      <c r="H23" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="47"/>
-      <c r="N23" s="16">
-        <f>N22-R22</f>
-        <v>3564.7058823529405</v>
-      </c>
-      <c r="O23" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="P23" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="8:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H24" s="41">
-        <f>H9+(N8+N23)/1000</f>
-        <v>6.325553319573439</v>
-      </c>
-      <c r="I24" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="P24" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="K4:K8"/>
+  <mergeCells count="7">
+    <mergeCell ref="E24:E28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="E4:E8"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q7 Q22">
+  <conditionalFormatting sqref="K7 K22">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>#REF!&lt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="K9" r:id="rId1"/>
+    <hyperlink ref="K24" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
electronic -> Schematic -> add hierarchical pins, modified Regulator page
           -> BOM & Clac: add new inductors
</commit_message>
<xml_diff>
--- a/Electronic/Design/Power_Calc.xlsx
+++ b/Electronic/Design/Power_Calc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>V</t>
   </si>
@@ -108,6 +108,15 @@
   </si>
   <si>
     <t>Max. 8.4V</t>
+  </si>
+  <si>
+    <t>22uH</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>15uH</t>
   </si>
 </sst>
 </file>
@@ -444,34 +453,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -575,6 +584,104 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>315007</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17887950" y="3876675"/>
+          <a:ext cx="4887007" cy="3000794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rechteck 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17954625" y="6524626"/>
+          <a:ext cx="3962400" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -845,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AH21" sqref="AH21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,24 +970,24 @@
     <col min="16" max="16" width="5.7109375" customWidth="1"/>
     <col min="17" max="17" width="4.28515625" customWidth="1"/>
     <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="55"/>
+    <col min="20" max="20" width="11.42578125" style="47"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="E4" s="51" t="s">
+      <c r="C4" s="51"/>
+      <c r="E4" s="48" t="s">
         <v>11</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="50"/>
+      <c r="K4" s="55"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -893,7 +1000,7 @@
       <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="52"/>
+      <c r="E5" s="49"/>
       <c r="H5" s="4">
         <v>6</v>
       </c>
@@ -921,7 +1028,7 @@
       <c r="R5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="55" t="s">
+      <c r="T5" s="47" t="s">
         <v>25</v>
       </c>
       <c r="U5" t="s">
@@ -937,7 +1044,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="E6" s="52"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="28"/>
       <c r="G6" s="14"/>
       <c r="H6" s="8">
@@ -973,6 +1080,12 @@
       <c r="R6" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="T6" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="U6" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="35">
@@ -982,7 +1095,7 @@
       <c r="C7" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="52"/>
+      <c r="E7" s="49"/>
       <c r="F7" s="29"/>
       <c r="H7" s="4">
         <f>L7*100/K6</f>
@@ -1017,7 +1130,7 @@
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="36"/>
       <c r="C8" s="9"/>
-      <c r="E8" s="52"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="30"/>
       <c r="H8" s="16">
         <f>H7-L7</f>
@@ -1059,7 +1172,7 @@
       <c r="J9" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="46" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1116,10 +1229,10 @@
       <c r="E19" s="27"/>
       <c r="F19" s="11"/>
       <c r="H19" s="1"/>
-      <c r="J19" s="49" t="s">
+      <c r="J19" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="50"/>
+      <c r="K19" s="55"/>
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1180,7 +1293,7 @@
       <c r="S21" t="s">
         <v>20</v>
       </c>
-      <c r="T21" s="55" t="s">
+      <c r="T21" s="47" t="s">
         <v>25</v>
       </c>
       <c r="U21">
@@ -1223,6 +1336,12 @@
       <c r="S22" t="s">
         <v>19</v>
       </c>
+      <c r="T22" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="U22" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F23" s="11"/>
@@ -1239,23 +1358,23 @@
       <c r="L23" s="1"/>
     </row>
     <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="51" t="s">
+      <c r="E24" s="48" t="s">
         <v>24</v>
       </c>
       <c r="F24" s="11"/>
       <c r="J24" t="s">
         <v>21</v>
       </c>
-      <c r="K24" s="54" t="s">
+      <c r="K24" s="46" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="E25" s="52"/>
+      <c r="C25" s="51"/>
+      <c r="E25" s="49"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1268,8 +1387,8 @@
       <c r="C26" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="52"/>
-      <c r="F26" s="53"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="34">
@@ -1280,7 +1399,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="15"/>
-      <c r="E27" s="52"/>
+      <c r="E27" s="49"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="35">
@@ -1290,7 +1409,7 @@
       <c r="C28" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E28" s="52"/>
+      <c r="E28" s="49"/>
     </row>
     <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="36"/>
@@ -1345,10 +1464,10 @@
     </row>
     <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="48"/>
+      <c r="C46" s="53"/>
     </row>
     <row r="47" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="41">

</xml_diff>

<commit_message>
Electronic: Power_Calc. updated & BOM add components
</commit_message>
<xml_diff>
--- a/Electronic/Design/Power_Calc.xlsx
+++ b/Electronic/Design/Power_Calc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5925"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -952,30 +952,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:U47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AH21" sqref="AH21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" customWidth="1"/>
-    <col min="13" max="13" width="4.28515625" customWidth="1"/>
-    <col min="14" max="14" width="4.7109375" customWidth="1"/>
-    <col min="15" max="15" width="4.140625" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="4.28515625" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" style="47"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="4.5546875" customWidth="1"/>
+    <col min="13" max="13" width="4.33203125" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" customWidth="1"/>
+    <col min="15" max="15" width="4.109375" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" customWidth="1"/>
+    <col min="17" max="17" width="4.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="47"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="50" t="s">
         <v>13</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="K4" s="55"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1035,10 +1035,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="34">
         <f>B7/B5</f>
-        <v>4.5391755532622398</v>
+        <v>4.5520410503382633</v>
       </c>
       <c r="C6" s="33" t="s">
         <v>14</v>
@@ -1049,7 +1049,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="8">
         <f>H7/H5</f>
-        <v>124.47368421052632</v>
+        <v>136.05263157894737</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>1</v>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="L6" s="12">
         <f>O5*P5+O6*P6+O7*P7+O8*P8</f>
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="M6" s="13" t="s">
         <v>1</v>
@@ -1087,10 +1087,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="35">
         <f>SUM(H7,H22)/(E10/100)/1000</f>
-        <v>27.235053319573439</v>
+        <v>27.312246302029578</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>15</v>
@@ -1099,7 +1099,7 @@
       <c r="F7" s="29"/>
       <c r="H7" s="4">
         <f>L7*100/K6</f>
-        <v>746.84210526315792</v>
+        <v>816.31578947368416</v>
       </c>
       <c r="I7" t="s">
         <v>2</v>
@@ -1108,7 +1108,7 @@
       <c r="K7" s="15"/>
       <c r="L7" s="7">
         <f>(L6*L5)</f>
-        <v>709.5</v>
+        <v>775.5</v>
       </c>
       <c r="M7" t="s">
         <v>2</v>
@@ -1127,14 +1127,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="36"/>
       <c r="C8" s="9"/>
       <c r="E8" s="49"/>
       <c r="F8" s="30"/>
       <c r="H8" s="16">
         <f>H7-L7</f>
-        <v>37.342105263157919</v>
+        <v>40.815789473684163</v>
       </c>
       <c r="I8" s="17" t="s">
         <v>2</v>
@@ -1145,7 +1145,7 @@
       <c r="L8" s="1"/>
       <c r="N8" s="11"/>
       <c r="O8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P8" s="2">
         <v>20</v>
@@ -1157,10 +1157,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B9" s="37">
         <f>B7-(H7+H22)/1000</f>
-        <v>2.723505331957341</v>
+        <v>2.7312246302029557</v>
       </c>
       <c r="C9" s="38" t="s">
         <v>16</v>
@@ -1176,7 +1176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E10" s="24">
         <v>90</v>
       </c>
@@ -1187,45 +1187,45 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E11" s="23"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
       <c r="E12" s="24"/>
       <c r="F12" s="30"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B13" s="40"/>
       <c r="C13" s="39"/>
       <c r="E13" s="25"/>
       <c r="F13" s="30"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="E14" s="23"/>
       <c r="F14" s="30"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E15" s="23"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E16" s="23"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E17" s="26"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E18" s="23"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E19" s="27"/>
       <c r="F19" s="11"/>
       <c r="H19" s="1"/>
@@ -1235,7 +1235,7 @@
       <c r="K19" s="55"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E20" t="s">
         <v>21</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F21" s="11"/>
       <c r="H21" s="19">
         <f>H22/H20</f>
@@ -1301,7 +1301,7 @@
         <v>5.8690476190476194E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F22" s="11"/>
       <c r="G22" s="44"/>
       <c r="H22" s="4">
@@ -1343,7 +1343,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F23" s="11"/>
       <c r="H23" s="16">
         <f>H22-L22</f>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E24" s="48" t="s">
         <v>24</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B25" s="50" t="s">
         <v>13</v>
       </c>
@@ -1377,7 +1377,7 @@
       <c r="E25" s="49"/>
       <c r="F25" s="11"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1390,10 +1390,10 @@
       <c r="E26" s="49"/>
       <c r="F26" s="45"/>
     </row>
-    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="34">
         <f>B28/B26</f>
-        <v>4.085257997936016</v>
+        <v>4.0968369453044371</v>
       </c>
       <c r="C27" s="33" t="s">
         <v>14</v>
@@ -1401,24 +1401,24 @@
       <c r="D27" s="15"/>
       <c r="E27" s="49"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B28" s="35">
         <f>SUM(H7,H22)/(E30/100)/1000</f>
-        <v>24.511547987616098</v>
+        <v>24.581021671826623</v>
       </c>
       <c r="C28" s="33" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="49"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="36"/>
       <c r="C29" s="9"/>
       <c r="E29" s="24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B30" s="37">
         <f>B28-(H7+H22)/1000</f>
         <v>0</v>
@@ -1430,49 +1430,49 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E31" s="23"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E32" s="24"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E33" s="25"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E34" s="23"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E35" s="23"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E36" s="23"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E37" s="26"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E38" s="23"/>
     </row>
-    <row r="39" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E39" s="27"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="52" t="s">
         <v>17</v>
       </c>
       <c r="C46" s="53"/>
     </row>
-    <row r="47" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="41">
         <f>B9+(H8+H23)/1000</f>
-        <v>6.325553319573439</v>
+        <v>6.3367463020295798</v>
       </c>
       <c r="C47" s="42" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Electronic: no charger, added Cp2102 instead of Ft232, first palcement
</commit_message>
<xml_diff>
--- a/Electronic/Design/Power_Calc.xlsx
+++ b/Electronic/Design/Power_Calc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5925"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>V</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Motors</t>
   </si>
   <si>
-    <t>Battery Charger &amp;                         Power Management</t>
-  </si>
-  <si>
     <t>Efficency</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>https://www.digikey.de/product-detail/de/analog-devices-inc/LT1374CS8-5-PBF/LT1374CS8-5-PBF-ND/888771</t>
   </si>
   <si>
-    <t>Battery &amp; Protection Circuit</t>
-  </si>
-  <si>
     <t xml:space="preserve">L = </t>
   </si>
   <si>
@@ -117,6 +111,15 @@
   </si>
   <si>
     <t>15uH</t>
+  </si>
+  <si>
+    <t>RGB-LED</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Battery Charger &amp; Protector +                        Power Management</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -453,7 +456,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -481,6 +483,29 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -558,8 +583,8 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>543506</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>163339</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1414</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -597,7 +622,7 @@
       <xdr:col>32</xdr:col>
       <xdr:colOff>315007</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>76619</xdr:rowOff>
+      <xdr:rowOff>105194</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -950,59 +975,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:U47"/>
+  <dimension ref="A3:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="5" width="14.44140625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
-    <col min="9" max="9" width="4.5546875" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" customWidth="1"/>
-    <col min="14" max="14" width="4.6640625" customWidth="1"/>
-    <col min="15" max="15" width="4.109375" customWidth="1"/>
-    <col min="16" max="16" width="5.6640625" customWidth="1"/>
-    <col min="17" max="17" width="4.33203125" customWidth="1"/>
-    <col min="18" max="18" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" style="47"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" customWidth="1"/>
+    <col min="15" max="15" width="4.140625" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" customWidth="1"/>
+    <col min="17" max="17" width="4.28515625" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" style="46"/>
     <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="E4" s="48" t="s">
-        <v>11</v>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="50"/>
+      <c r="E4" s="47" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="J4" s="54" t="s">
+      <c r="J4" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="55"/>
+      <c r="K4" s="54"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="48"/>
       <c r="H5" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I5" t="s">
         <v>0</v>
@@ -1028,40 +1057,40 @@
       <c r="R5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="47" t="s">
-        <v>25</v>
+      <c r="T5" s="46" t="s">
+        <v>23</v>
       </c>
       <c r="U5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="34">
         <f>B7/B5</f>
-        <v>4.5520410503382633</v>
+        <v>4.1108152734778125</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="15"/>
-      <c r="E6" s="49"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="28"/>
       <c r="G6" s="14"/>
       <c r="H6" s="8">
         <f>H7/H5</f>
-        <v>136.05263157894737</v>
+        <v>163.26315789473682</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" s="11">
         <v>95</v>
       </c>
       <c r="L6" s="12">
-        <f>O5*P5+O6*P6+O7*P7+O8*P8</f>
+        <f>O5*P5+O6*P6+O23*P23+O7*P7</f>
         <v>235</v>
       </c>
       <c r="M6" s="13" t="s">
@@ -1080,22 +1109,22 @@
       <c r="R6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="T6" s="47" t="s">
-        <v>29</v>
+      <c r="T6" s="46" t="s">
+        <v>27</v>
       </c>
       <c r="U6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="35">
         <f>SUM(H7,H22)/(E10/100)/1000</f>
-        <v>27.312246302029578</v>
+        <v>20.554076367389062</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="49"/>
+        <v>14</v>
+      </c>
+      <c r="E7" s="48"/>
       <c r="F7" s="29"/>
       <c r="H7" s="4">
         <f>L7*100/K6</f>
@@ -1115,7 +1144,7 @@
       </c>
       <c r="N7" s="11"/>
       <c r="O7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P7" s="2">
         <v>20</v>
@@ -1124,13 +1153,13 @@
         <v>1</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="36"/>
       <c r="C8" s="9"/>
-      <c r="E8" s="49"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="30"/>
       <c r="H8" s="16">
         <f>H7-L7</f>
@@ -1144,39 +1173,27 @@
       </c>
       <c r="L8" s="1"/>
       <c r="N8" s="11"/>
-      <c r="O8">
-        <v>5</v>
-      </c>
-      <c r="P8" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="37">
         <f>B7-(H7+H22)/1000</f>
-        <v>2.7312246302029557</v>
+        <v>2.0554076367389058</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="30"/>
       <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="46" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10" s="24">
         <v>90</v>
       </c>
@@ -1187,57 +1204,57 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E11" s="23"/>
       <c r="F11" s="30"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
       <c r="E12" s="24"/>
       <c r="F12" s="30"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="40"/>
       <c r="C13" s="39"/>
       <c r="E13" s="25"/>
       <c r="F13" s="30"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="E14" s="23"/>
       <c r="F14" s="30"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E15" s="23"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E16" s="23"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E17" s="26"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E18" s="23"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E19" s="27"/>
       <c r="F19" s="11"/>
       <c r="H19" s="1"/>
-      <c r="J19" s="54" t="s">
+      <c r="J19" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="55"/>
+      <c r="K19" s="54"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="11"/>
       <c r="H20" s="4">
@@ -1255,24 +1272,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F21" s="11"/>
       <c r="H21" s="19">
         <f>H22/H20</f>
-        <v>3960.7843137254899</v>
+        <v>2947.0588235294122</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>1</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K21" s="11">
         <v>85</v>
       </c>
       <c r="L21" s="20">
-        <f>(P21*O21+P22*O22)</f>
-        <v>4040</v>
+        <f>(P21*O21+P22*O22+O23*P23+O24*P24)</f>
+        <v>3006</v>
       </c>
       <c r="M21" s="13" t="s">
         <v>1</v>
@@ -1282,7 +1299,7 @@
         <v>2</v>
       </c>
       <c r="P21" s="21">
-        <v>1920</v>
+        <v>1333</v>
       </c>
       <c r="Q21" t="s">
         <v>1</v>
@@ -1291,22 +1308,22 @@
         <v>10</v>
       </c>
       <c r="S21" t="s">
-        <v>20</v>
-      </c>
-      <c r="T21" s="47" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="T21" s="46" t="s">
+        <v>23</v>
       </c>
       <c r="U21">
         <f>(0.29*L20*(H20+2.4-L20))/(0.2*500000*(H20+2.4))</f>
         <v>5.8690476190476194E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F22" s="11"/>
+    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="31"/>
       <c r="G22" s="44"/>
       <c r="H22" s="4">
         <f>L22*100/K21</f>
-        <v>23764.705882352941</v>
+        <v>17682.352941176472</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>2</v>
@@ -1315,7 +1332,7 @@
       <c r="K22" s="15"/>
       <c r="L22" s="7">
         <f>L21*L20</f>
-        <v>20200</v>
+        <v>15030</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>2</v>
@@ -1331,23 +1348,23 @@
         <v>1</v>
       </c>
       <c r="R22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S22" t="s">
         <v>18</v>
       </c>
-      <c r="S22" t="s">
-        <v>19</v>
-      </c>
-      <c r="T22" s="47" t="s">
-        <v>29</v>
+      <c r="T22" s="46" t="s">
+        <v>27</v>
       </c>
       <c r="U22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F23" s="11"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F23" s="31"/>
       <c r="H23" s="16">
         <f>H22-L22</f>
-        <v>3564.7058823529405</v>
+        <v>2652.3529411764721</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>2</v>
@@ -1356,134 +1373,167 @@
         <v>3</v>
       </c>
       <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23">
+        <v>4</v>
+      </c>
+      <c r="P23" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="31"/>
       <c r="J24" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="51"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="11"/>
-    </row>
-    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="32">
-        <v>6</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="45"/>
-    </row>
-    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="34">
-        <f>B28/B26</f>
-        <v>4.0968369453044371</v>
-      </c>
-      <c r="C27" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="N24" s="11"/>
+      <c r="O24">
+        <v>1</v>
+      </c>
+      <c r="P24" s="2">
+        <v>60</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="31"/>
+      <c r="K25" s="45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="59"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="31"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="59"/>
+      <c r="B27" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="52"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="65"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="59"/>
+      <c r="B28" s="41">
+        <f>B9+(H8+H23)/1000</f>
+        <v>4.7485763673890622</v>
+      </c>
+      <c r="C28" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="49"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B28" s="35">
-        <f>SUM(H7,H22)/(E30/100)/1000</f>
-        <v>24.581021671826623</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="49"/>
-    </row>
-    <row r="29" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="36"/>
-      <c r="C29" s="9"/>
-      <c r="E29" s="24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B30" s="37">
-        <f>B28-(H7+H22)/1000</f>
-        <v>0</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E31" s="23"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E33" s="25"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E34" s="23"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E35" s="23"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E36" s="23"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E37" s="26"/>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E38" s="23"/>
-    </row>
-    <row r="39" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E39" s="27"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E40" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B46" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="C46" s="53"/>
-    </row>
-    <row r="47" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="41">
-        <f>B9+(H8+H23)/1000</f>
-        <v>6.3367463020295798</v>
-      </c>
-      <c r="C47" s="42" t="s">
-        <v>15</v>
-      </c>
+      <c r="D28" s="59"/>
+      <c r="E28" s="65"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="59"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="61"/>
+      <c r="O29" s="31"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="59"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="61"/>
+      <c r="O30" s="31"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="59"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="62"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="59"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="61"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="59"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="63"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="59"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="62"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="59"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="62"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="59"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="62"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="59"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="64"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="59"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="62"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="59"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="E24:E28"/>
-    <mergeCell ref="B25:C25"/>
+  <mergeCells count="5">
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="E4:E8"/>
@@ -1495,7 +1545,7 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K9" r:id="rId1"/>
-    <hyperlink ref="K24" r:id="rId2"/>
+    <hyperlink ref="K25" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>